<commit_message>
invalid ids, department wise books
</commit_message>
<xml_diff>
--- a/OUTPUT/ChartBook.xlsx
+++ b/OUTPUT/ChartBook.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="III year" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="III year" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -125,13 +125,13 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -154,7 +154,7 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>5</col>
@@ -197,9 +197,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -492,7 +492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -540,13 +540,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C2" t="n">
         <v>181</v>
       </c>
       <c r="D2" t="n">
-        <v>69.61</v>
+        <v>70.72</v>
       </c>
     </row>
     <row r="3">
@@ -647,6 +647,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>